<commit_message>
Update XGBoost Change Prediction
</commit_message>
<xml_diff>
--- a/Data/Predictions/XGBoost/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
+++ b/Data/Predictions/XGBoost/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
@@ -635,7 +635,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3535,7 +3535,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4615,7 +4615,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5795,7 +5795,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6255,7 +6255,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6315,7 +6315,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6355,7 +6355,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6675,7 +6675,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6695,7 +6695,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7775,7 +7775,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8015,7 +8015,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8115,7 +8115,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8675,7 +8675,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8895,7 +8895,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9035,7 +9035,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9315,7 +9315,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9495,7 +9495,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9775,7 +9775,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9855,7 +9855,7 @@
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9935,7 +9935,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10215,7 +10215,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10615,7 +10615,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10675,7 +10675,7 @@
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10735,7 +10735,7 @@
       </c>
       <c r="D515" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11035,7 +11035,7 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11075,7 +11075,7 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11315,7 +11315,7 @@
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11475,7 +11475,7 @@
       </c>
       <c r="D552" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11535,7 +11535,7 @@
       </c>
       <c r="D555" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11575,7 +11575,7 @@
       </c>
       <c r="D557" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="D569" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11915,7 +11915,7 @@
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12075,7 +12075,7 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12375,7 +12375,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12715,7 +12715,7 @@
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12735,7 +12735,7 @@
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="D617" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12855,7 +12855,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13115,7 +13115,7 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13135,7 +13135,7 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13195,7 +13195,7 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13415,7 +13415,7 @@
       </c>
       <c r="D649" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13435,7 +13435,7 @@
       </c>
       <c r="D650" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13735,7 +13735,7 @@
       </c>
       <c r="D665" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13815,7 +13815,7 @@
       </c>
       <c r="D669" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13995,7 +13995,7 @@
       </c>
       <c r="D678" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14035,7 +14035,7 @@
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14075,7 +14075,7 @@
       </c>
       <c r="D682" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14095,7 +14095,7 @@
       </c>
       <c r="D683" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14155,7 +14155,7 @@
       </c>
       <c r="D686" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14195,7 +14195,7 @@
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14655,7 +14655,7 @@
       </c>
       <c r="D711" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14955,7 +14955,7 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15355,7 +15355,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15575,7 +15575,7 @@
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15615,7 +15615,7 @@
       </c>
       <c r="D759" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="D768" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15835,7 +15835,7 @@
       </c>
       <c r="D770" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15955,7 +15955,7 @@
       </c>
       <c r="D776" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="D785" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16235,7 +16235,7 @@
       </c>
       <c r="D790" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16275,7 +16275,7 @@
       </c>
       <c r="D792" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16695,7 +16695,7 @@
       </c>
       <c r="D813" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16835,7 +16835,7 @@
       </c>
       <c r="D820" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="D822" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17135,7 +17135,7 @@
       </c>
       <c r="D835" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17255,7 +17255,7 @@
       </c>
       <c r="D841" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17355,7 +17355,7 @@
       </c>
       <c r="D846" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17375,7 +17375,7 @@
       </c>
       <c r="D847" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="D851" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17655,7 +17655,7 @@
       </c>
       <c r="D861" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17755,7 +17755,7 @@
       </c>
       <c r="D866" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="D876" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18015,7 +18015,7 @@
       </c>
       <c r="D879" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18135,7 +18135,7 @@
       </c>
       <c r="D885" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18235,7 +18235,7 @@
       </c>
       <c r="D890" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="D894" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18355,7 +18355,7 @@
       </c>
       <c r="D896" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18395,7 +18395,7 @@
       </c>
       <c r="D898" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18415,7 +18415,7 @@
       </c>
       <c r="D899" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18635,7 +18635,7 @@
       </c>
       <c r="D910" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="D914" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18815,7 +18815,7 @@
       </c>
       <c r="D919" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18855,7 +18855,7 @@
       </c>
       <c r="D921" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18955,7 +18955,7 @@
       </c>
       <c r="D926" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19155,7 +19155,7 @@
       </c>
       <c r="D936" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19195,7 +19195,7 @@
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19355,7 +19355,7 @@
       </c>
       <c r="D946" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19395,7 +19395,7 @@
       </c>
       <c r="D948" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19515,7 +19515,7 @@
       </c>
       <c r="D954" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19715,7 +19715,7 @@
       </c>
       <c r="D964" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19755,7 +19755,7 @@
       </c>
       <c r="D966" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19955,7 +19955,7 @@
       </c>
       <c r="D976" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19995,7 +19995,7 @@
       </c>
       <c r="D978" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20015,7 +20015,7 @@
       </c>
       <c r="D979" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20455,7 +20455,7 @@
       </c>
       <c r="D1001" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20535,7 +20535,7 @@
       </c>
       <c r="D1005" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20635,7 +20635,7 @@
       </c>
       <c r="D1010" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20795,7 +20795,7 @@
       </c>
       <c r="D1018" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20815,7 +20815,7 @@
       </c>
       <c r="D1019" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20995,7 +20995,7 @@
       </c>
       <c r="D1028" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21235,7 +21235,7 @@
       </c>
       <c r="D1040" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21335,7 +21335,7 @@
       </c>
       <c r="D1045" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21495,7 +21495,7 @@
       </c>
       <c r="D1053" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21515,7 +21515,7 @@
       </c>
       <c r="D1054" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21535,7 +21535,7 @@
       </c>
       <c r="D1055" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21615,7 +21615,7 @@
       </c>
       <c r="D1059" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21755,7 +21755,7 @@
       </c>
       <c r="D1066" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21835,7 +21835,7 @@
       </c>
       <c r="D1070" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22015,7 +22015,7 @@
       </c>
       <c r="D1079" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22055,7 +22055,7 @@
       </c>
       <c r="D1081" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22195,7 +22195,7 @@
       </c>
       <c r="D1088" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22255,7 +22255,7 @@
       </c>
       <c r="D1091" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22295,7 +22295,7 @@
       </c>
       <c r="D1093" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22315,7 +22315,7 @@
       </c>
       <c r="D1094" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22355,7 +22355,7 @@
       </c>
       <c r="D1096" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22375,7 +22375,7 @@
       </c>
       <c r="D1097" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22455,7 +22455,7 @@
       </c>
       <c r="D1101" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22475,7 +22475,7 @@
       </c>
       <c r="D1102" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22495,7 +22495,7 @@
       </c>
       <c r="D1103" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22555,7 +22555,7 @@
       </c>
       <c r="D1106" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22815,7 +22815,7 @@
       </c>
       <c r="D1119" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>

</xml_diff>